<commit_message>
Fixed deck adjustment bug
</commit_message>
<xml_diff>
--- a/MVPlate/MV_InputTemplate.xlsx
+++ b/MVPlate/MV_InputTemplate.xlsx
@@ -603,7 +603,7 @@
   <dimension ref="A1:O64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,7 +722,7 @@
         <v>30</v>
       </c>
       <c r="F6" s="10">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H6" s="9"/>
       <c r="N6" s="9" t="s">

</xml_diff>

<commit_message>
Accepting either comma delimiter for MVplate
</commit_message>
<xml_diff>
--- a/MVPlate/MV_InputTemplate.xlsx
+++ b/MVPlate/MV_InputTemplate.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="38">
   <si>
     <t>Drug Name</t>
   </si>
@@ -160,6 +160,15 @@
   </si>
   <si>
     <t>AB4</t>
+  </si>
+  <si>
+    <t>, s</t>
+  </si>
+  <si>
+    <t>64,5</t>
+  </si>
+  <si>
+    <t>1000,5</t>
   </si>
 </sst>
 </file>
@@ -603,7 +612,7 @@
   <dimension ref="A1:O64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,8 +650,8 @@
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6">
-        <v>1000</v>
+      <c r="C2" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="D2" s="6">
         <v>1000</v>
@@ -724,7 +733,9 @@
       <c r="F6" s="10">
         <v>2</v>
       </c>
-      <c r="H6" s="9"/>
+      <c r="H6" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="N6" s="9" t="s">
         <v>22</v>
       </c>
@@ -1128,22 +1139,21 @@
       <c r="F22" s="2">
         <v>128</v>
       </c>
-      <c r="G22" s="2">
-        <f t="shared" ref="G22:G27" si="1">F22/2</f>
-        <v>64</v>
+      <c r="G22" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="H22" s="2">
         <v>128</v>
       </c>
       <c r="I22" s="2">
-        <f t="shared" ref="I22:I27" si="2">H22/2</f>
+        <f t="shared" ref="I22:I27" si="1">H22/2</f>
         <v>64</v>
       </c>
       <c r="J22" s="2">
         <v>128</v>
       </c>
       <c r="K22" s="2">
-        <f t="shared" ref="K22:K27" si="3">J22/2</f>
+        <f t="shared" ref="K22:K27" si="2">J22/2</f>
         <v>64</v>
       </c>
       <c r="L22" s="2">
@@ -1176,22 +1186,21 @@
       <c r="F23" s="2">
         <v>128</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H23" s="2">
+        <v>128</v>
+      </c>
+      <c r="I23" s="2">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="H23" s="2">
-        <v>128</v>
-      </c>
-      <c r="I23" s="2">
-        <f t="shared" si="2"/>
-        <v>64</v>
-      </c>
       <c r="J23" s="2">
         <v>128</v>
       </c>
       <c r="K23" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="L23" s="2">
@@ -1221,22 +1230,21 @@
       <c r="F24" s="2">
         <v>128</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H24" s="2">
+        <v>128</v>
+      </c>
+      <c r="I24" s="2">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="H24" s="2">
-        <v>128</v>
-      </c>
-      <c r="I24" s="2">
-        <f t="shared" si="2"/>
-        <v>64</v>
-      </c>
       <c r="J24" s="2">
         <v>128</v>
       </c>
       <c r="K24" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="L24" s="2">
@@ -1266,22 +1274,21 @@
       <c r="F25" s="2">
         <v>128</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H25" s="2">
+        <v>128</v>
+      </c>
+      <c r="I25" s="2">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="H25" s="2">
-        <v>128</v>
-      </c>
-      <c r="I25" s="2">
-        <f t="shared" si="2"/>
-        <v>64</v>
-      </c>
       <c r="J25" s="2">
         <v>128</v>
       </c>
       <c r="K25" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="L25" s="2">
@@ -1311,22 +1318,21 @@
       <c r="F26" s="2">
         <v>128</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H26" s="2">
+        <v>128</v>
+      </c>
+      <c r="I26" s="2">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="H26" s="2">
-        <v>128</v>
-      </c>
-      <c r="I26" s="2">
-        <f t="shared" si="2"/>
-        <v>64</v>
-      </c>
       <c r="J26" s="2">
         <v>128</v>
       </c>
       <c r="K26" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="L26" s="2">
@@ -1356,22 +1362,21 @@
       <c r="F27" s="2">
         <v>128</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H27" s="2">
+        <v>128</v>
+      </c>
+      <c r="I27" s="2">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="H27" s="2">
-        <v>128</v>
-      </c>
-      <c r="I27" s="2">
-        <f t="shared" si="2"/>
-        <v>64</v>
-      </c>
       <c r="J27" s="2">
         <v>128</v>
       </c>
       <c r="K27" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="L27" s="2">
@@ -2144,47 +2149,47 @@
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="C57" s="4" t="str">
-        <f t="shared" ref="C57:M57" si="4">CONCATENATE(C10," ",C21," ",C33," ",C45)</f>
+        <f t="shared" ref="C57:M57" si="3">CONCATENATE(C10," ",C21," ",C33," ",C45)</f>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="D57" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="E57" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="F57" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="G57" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="H57" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="I57" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="J57" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="K57" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="L57" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="M57" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
     </row>
@@ -2193,51 +2198,51 @@
         <v>6</v>
       </c>
       <c r="B58" s="4" t="str">
-        <f t="shared" ref="B58:M64" si="5">CONCATENATE(B11," ",B22," ",B34," ",B46)</f>
+        <f t="shared" ref="B58:M64" si="4">CONCATENATE(B11," ",B22," ",B34," ",B46)</f>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="C58" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A STR_A</v>
       </c>
       <c r="D58" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB1 128 MED_A STR_A</v>
       </c>
       <c r="E58" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB1 64 MED_A STR_A</v>
       </c>
       <c r="F58" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB2 128 MED_A STR_A</v>
       </c>
       <c r="G58" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>AB2 64 MED_A STR_A</v>
+        <f t="shared" si="4"/>
+        <v>AB2 64,5 MED_A STR_A</v>
       </c>
       <c r="H58" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB3 128 MED_A STR_A</v>
       </c>
       <c r="I58" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB3 64 MED_A STR_A</v>
       </c>
       <c r="J58" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB4 128 MED_A STR_A</v>
       </c>
       <c r="K58" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB4 64 MED_A STR_A</v>
       </c>
       <c r="L58" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="M58" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
     </row>
@@ -2246,51 +2251,51 @@
         <v>7</v>
       </c>
       <c r="B59" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="C59" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A STR_A</v>
       </c>
       <c r="D59" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB1 128 MED_A STR_A</v>
       </c>
       <c r="E59" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB1 64 MED_A STR_A</v>
       </c>
       <c r="F59" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB2 128 MED_A STR_A</v>
       </c>
       <c r="G59" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>AB2 64 MED_A STR_A</v>
+        <f t="shared" si="4"/>
+        <v>AB2 64,5 MED_A STR_A</v>
       </c>
       <c r="H59" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB3 128 MED_A STR_A</v>
       </c>
       <c r="I59" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB3 64 MED_A STR_A</v>
       </c>
       <c r="J59" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB4 128 MED_A STR_A</v>
       </c>
       <c r="K59" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB4 64 MED_A STR_A</v>
       </c>
       <c r="L59" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="M59" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
     </row>
@@ -2299,51 +2304,51 @@
         <v>8</v>
       </c>
       <c r="B60" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="C60" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A STR_A</v>
       </c>
       <c r="D60" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB1 128 MED_A STR_A</v>
       </c>
       <c r="E60" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB1 64 MED_A STR_A</v>
       </c>
       <c r="F60" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB2 128 MED_A STR_A</v>
       </c>
       <c r="G60" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>AB2 64 MED_A STR_A</v>
+        <f t="shared" si="4"/>
+        <v>AB2 64,5 MED_A STR_A</v>
       </c>
       <c r="H60" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB3 128 MED_A STR_A</v>
       </c>
       <c r="I60" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB3 64 MED_A STR_A</v>
       </c>
       <c r="J60" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB4 128 MED_A STR_A</v>
       </c>
       <c r="K60" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB4 64 MED_A STR_A</v>
       </c>
       <c r="L60" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="M60" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
     </row>
@@ -2352,51 +2357,51 @@
         <v>9</v>
       </c>
       <c r="B61" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="C61" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A STR_B</v>
       </c>
       <c r="D61" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB1 128 MED_A STR_B</v>
       </c>
       <c r="E61" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB1 64 MED_A STR_B</v>
       </c>
       <c r="F61" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB2 128 MED_A STR_B</v>
       </c>
       <c r="G61" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>AB2 64 MED_A STR_B</v>
+        <f t="shared" si="4"/>
+        <v>AB2 64,5 MED_A STR_B</v>
       </c>
       <c r="H61" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB3 128 MED_A STR_B</v>
       </c>
       <c r="I61" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB3 64 MED_A STR_B</v>
       </c>
       <c r="J61" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB4 128 MED_A STR_B</v>
       </c>
       <c r="K61" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB4 64 MED_A STR_B</v>
       </c>
       <c r="L61" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="M61" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
     </row>
@@ -2405,51 +2410,51 @@
         <v>10</v>
       </c>
       <c r="B62" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="C62" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A STR_B</v>
       </c>
       <c r="D62" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB1 128 MED_A STR_B</v>
       </c>
       <c r="E62" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB1 64 MED_A STR_B</v>
       </c>
       <c r="F62" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB2 128 MED_A STR_B</v>
       </c>
       <c r="G62" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>AB2 64 MED_A STR_B</v>
+        <f t="shared" si="4"/>
+        <v>AB2 64,5 MED_A STR_B</v>
       </c>
       <c r="H62" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB3 128 MED_A STR_B</v>
       </c>
       <c r="I62" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB3 64 MED_A STR_B</v>
       </c>
       <c r="J62" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB4 128 MED_A STR_B</v>
       </c>
       <c r="K62" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB4 64 MED_A STR_B</v>
       </c>
       <c r="L62" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="M62" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
     </row>
@@ -2458,51 +2463,51 @@
         <v>11</v>
       </c>
       <c r="B63" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="C63" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A STR_B</v>
       </c>
       <c r="D63" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB1 128 MED_A STR_B</v>
       </c>
       <c r="E63" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB1 64 MED_A STR_B</v>
       </c>
       <c r="F63" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB2 128 MED_A STR_B</v>
       </c>
       <c r="G63" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>AB2 64 MED_A STR_B</v>
+        <f t="shared" si="4"/>
+        <v>AB2 64,5 MED_A STR_B</v>
       </c>
       <c r="H63" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB3 128 MED_A STR_B</v>
       </c>
       <c r="I63" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB3 64 MED_A STR_B</v>
       </c>
       <c r="J63" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB4 128 MED_A STR_B</v>
       </c>
       <c r="K63" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>AB4 64 MED_A STR_B</v>
       </c>
       <c r="L63" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="M63" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
     </row>
@@ -2511,51 +2516,51 @@
         <v>12</v>
       </c>
       <c r="B64" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="C64" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="D64" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="E64" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="F64" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="G64" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="H64" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="I64" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="J64" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="K64" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="L64" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
       <c r="M64" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> 0 MED_A </v>
       </c>
     </row>

</xml_diff>